<commit_message>
30 on, 30 off continuous pulse protocol
</commit_message>
<xml_diff>
--- a/protocol_shortdutycycle_20190807.xlsx
+++ b/protocol_shortdutycycle_20190807.xlsx
@@ -368,7 +368,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,13 +420,13 @@
         <v>30</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>30000</v>
       </c>
       <c r="D2">
-        <v>25</v>
+        <v>30000</v>
       </c>
       <c r="E2">
-        <v>1200</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>30000</v>
@@ -450,13 +450,13 @@
         <v>60</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>30000</v>
       </c>
       <c r="D3">
-        <v>25</v>
+        <v>30000</v>
       </c>
       <c r="E3">
-        <v>1200</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>30000</v>

</xml_diff>